<commit_message>
added KEGG table for the MS
</commit_message>
<xml_diff>
--- a/RAnalysis/Output/WGCNA/KEGG_summary_table.xlsx
+++ b/RAnalysis/Output/WGCNA/KEGG_summary_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Cvirginica_multistressor\RAnalysis\Output\WGCNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2762594-FD9F-4D00-AD59-E945F55DC8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1786AAD-7BB8-4BE8-B2F9-D8E22C161768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21855" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clusterProfiler_KEGG" sheetId="3" r:id="rId1"/>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047AA346-6573-4D3C-937B-7CE03BF1F377}">
   <dimension ref="A1:X868"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45541,7 +45541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X932"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B43" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>

</xml_diff>